<commit_message>
(web) Cleaned supp. data files; updated dataset 9
- updated supplementary data 9, as it includes a pretty important fix
</commit_message>
<xml_diff>
--- a/supplementary_data/supplementary_data_1.xlsx
+++ b/supplementary_data/supplementary_data_1.xlsx
@@ -2,13 +2,8 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
-  <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\team\lapt3u\projects\side\viral_titer\manuscript\_nature_comm_med_version\reviews\_editorial_resubmission\Supplementary Data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52783CAA-98FD-4AC4-85E4-1BCE696CAA3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="202300"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAA2928D-06DB-4C0F-B3A0-85282A31F06D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{F54BBE4F-620C-4FE4-BD3C-9E35CF942F7F}"/>
   </bookViews>
@@ -920,6 +915,7 @@
     <mergeCell ref="A2:G9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Minor supplementary data updates (…)
Also updated the README to mention Batch Purifier, a commercial metadata
scrubber.
</commit_message>
<xml_diff>
--- a/supplementary_data/supplementary_data_1.xlsx
+++ b/supplementary_data/supplementary_data_1.xlsx
@@ -2,8 +2,11 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="202300"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAA2928D-06DB-4C0F-B3A0-85282A31F06D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookPr defaultThemeVersion="202300" filterPrivacy="1"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15"/>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52783CAA-98FD-4AC4-85E4-1BCE696CAA3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{F54BBE4F-620C-4FE4-BD3C-9E35CF942F7F}"/>
   </bookViews>
@@ -915,7 +918,6 @@
     <mergeCell ref="A2:G9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>